<commit_message>
feat(main): Implemented Issue #5, #6 and #8
Along with the implemented issues, I also added a few new "handler" classes to simplify the code.
</commit_message>
<xml_diff>
--- a/T-P_POO-NeoDarbellay.xlsx
+++ b/T-P_POO-NeoDarbellay.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\Vacances\P_POO-I320\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0BCE75-E1C4-40D7-943A-52B6C788B70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D97C530-466F-4051-A93F-47CEC88C1536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1176" yWindow="0" windowWidth="21960" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
     <sheet name="Restrictions" sheetId="19" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$70</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="98">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -323,6 +323,30 @@
   </si>
   <si>
     <t>Installation of Github Desktop</t>
+  </si>
+  <si>
+    <t>Committing everything to GitHub</t>
+  </si>
+  <si>
+    <t>Github Desktop</t>
+  </si>
+  <si>
+    <t>Created a commit to add every file to GitHub</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>Took a small break and started again at 17:05</t>
+  </si>
+  <si>
+    <t>Implementation of Issue #6 to the program</t>
+  </si>
+  <si>
+    <t>Implementation of Issue #8 to the program</t>
+  </si>
+  <si>
+    <t>Took a 30 minute break in between to go eat</t>
   </si>
 </sst>
 </file>
@@ -699,7 +723,21 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1094,26 +1132,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="50.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="36" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="10" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1224,7 +1262,7 @@
       </c>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
@@ -1930,7 +1968,9 @@
         <v>31</v>
       </c>
       <c r="B43" s="28"/>
-      <c r="C43" s="26"/>
+      <c r="C43" s="26">
+        <v>15</v>
+      </c>
       <c r="D43" s="8" t="s">
         <v>87</v>
       </c>
@@ -1947,116 +1987,174 @@
         <v>88</v>
       </c>
       <c r="B44" s="28"/>
-      <c r="C44" s="26"/>
+      <c r="C44" s="26">
+        <v>10</v>
+      </c>
       <c r="D44" s="8" t="s">
         <v>89</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" s="23"/>
-      <c r="G44" s="19"/>
-    </row>
-    <row r="45" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F44" s="23">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>53</v>
       </c>
       <c r="B45" s="28"/>
-      <c r="C45" s="26"/>
+      <c r="C45" s="26">
+        <v>25</v>
+      </c>
       <c r="D45" s="8" t="s">
         <v>84</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" s="23"/>
-      <c r="G45" s="19"/>
+        <v>32</v>
+      </c>
+      <c r="F45" s="23">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="29"/>
+      <c r="C46" s="26">
+        <v>5</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="23">
+        <v>0.72569444444444442</v>
+      </c>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B47" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C47" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="38">
+      <c r="D47" s="38">
         <f>SUM(C36:C45)</f>
-        <v>185</v>
-      </c>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="39"/>
-    </row>
-    <row r="47" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="19"/>
+        <v>235</v>
+      </c>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="19"/>
+      <c r="A48" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="27">
+        <v>45954</v>
+      </c>
+      <c r="C48" s="5">
+        <v>70</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" s="23">
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B49" s="28"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="7"/>
+      <c r="C49" s="7">
+        <v>85</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" s="23">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="G49" s="19"/>
     </row>
-    <row r="50" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+    <row r="50" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B50" s="28"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="19"/>
+      <c r="C50" s="7">
+        <v>170</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="23">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="19"/>
-    </row>
-    <row r="52" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
+      <c r="A51" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B51" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C51" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D52" s="38">
-        <f>SUM(C47:C51)</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="39"/>
+      <c r="D51" s="38">
+        <f>SUM(C48:C50)</f>
+        <v>325</v>
+      </c>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="39"/>
+    </row>
+    <row r="52" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="19"/>
     </row>
     <row r="53" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="5"/>
+      <c r="A53" s="6"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="22"/>
@@ -2068,7 +2166,7 @@
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
-      <c r="F54" s="22"/>
+      <c r="F54" s="7"/>
       <c r="G54" s="19"/>
     </row>
     <row r="55" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2080,46 +2178,46 @@
       <c r="F55" s="7"/>
       <c r="G55" s="19"/>
     </row>
-    <row r="56" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="28"/>
-      <c r="C56" s="7"/>
+    <row r="56" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="9"/>
       <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+      <c r="E56" s="10"/>
       <c r="F56" s="7"/>
       <c r="G56" s="19"/>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="19"/>
-    </row>
-    <row r="58" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="11" t="s">
+      <c r="A57" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B57" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C57" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="38">
-        <f>SUM(C53:C57)</f>
+      <c r="D57" s="38">
+        <f>SUM(C52:C56)</f>
         <v>0</v>
       </c>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="39"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="39"/>
+    </row>
+    <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="5"/>
+      <c r="A59" s="6"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="7"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="22"/>
@@ -2131,7 +2229,7 @@
       <c r="C60" s="7"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
-      <c r="F60" s="22"/>
+      <c r="F60" s="7"/>
       <c r="G60" s="19"/>
     </row>
     <row r="61" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2143,46 +2241,46 @@
       <c r="F61" s="7"/>
       <c r="G61" s="19"/>
     </row>
-    <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="28"/>
-      <c r="C62" s="7"/>
+    <row r="62" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="9"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="9"/>
       <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
+      <c r="E62" s="10"/>
       <c r="F62" s="7"/>
       <c r="G62" s="19"/>
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
-      <c r="B63" s="29"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="19"/>
-    </row>
-    <row r="64" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="11" t="s">
+      <c r="A63" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B63" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C63" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="38">
-        <f>SUM(C59:C63)</f>
+      <c r="D63" s="38">
+        <f>SUM(C58:C62)</f>
         <v>0</v>
       </c>
-      <c r="E64" s="38"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="39"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="39"/>
+    </row>
+    <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="19"/>
     </row>
     <row r="65" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="5"/>
+      <c r="A65" s="6"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="7"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="22"/>
@@ -2194,7 +2292,7 @@
       <c r="C66" s="7"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
-      <c r="F66" s="22"/>
+      <c r="F66" s="7"/>
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2206,78 +2304,64 @@
       <c r="F67" s="7"/>
       <c r="G67" s="19"/>
     </row>
-    <row r="68" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="28"/>
-      <c r="C68" s="7"/>
+    <row r="68" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="9"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="9"/>
       <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
+      <c r="E68" s="10"/>
       <c r="F68" s="7"/>
       <c r="G68" s="19"/>
     </row>
     <row r="69" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
-      <c r="B69" s="29"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="19"/>
-    </row>
-    <row r="70" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="11" t="s">
+      <c r="A69" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B69" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C70" s="17" t="s">
+      <c r="C69" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D70" s="38">
-        <f>SUM(C65:C69)</f>
+      <c r="D69" s="38">
+        <f>SUM(C64:C68)</f>
         <v>0</v>
       </c>
-      <c r="E70" s="38"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="39"/>
-    </row>
-    <row r="71" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="30" t="s">
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="39"/>
+    </row>
+    <row r="70" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="31"/>
-      <c r="C71" s="12">
-        <f>MROUND(SUM(C6:C70) /60,0.2)</f>
-        <v>12.4</v>
-      </c>
-      <c r="D71" s="13"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="14"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="12">
+        <f>MROUND(SUM(C6:C69) /60,0.2)</f>
+        <v>18.8</v>
+      </c>
+      <c r="D70" s="13"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="14"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
+      <c r="A72" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="D64:G64"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="D69:G69"/>
     <mergeCell ref="B19:B34"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="B36:B46"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -2287,19 +2371,24 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B36:B45"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="B64:B68"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C65:C69 C53:C57 C59:C63 C6:C11 B6 C13:C17 C36:C45 C47:C51 C19:C34" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C64:C68 C52:C56 C58:C62 C6:C11 B6 C13:C17 C19:C34 C48:C50 C36:C46" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B13:B17 B65:B69 B36:B45 B47:B51 B53:B57 B59:B63 B19:B34" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B13:B17 B64:B68 B19:B34 B48:B50 B52:B56 B58:B62 B36" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -2318,7 +2407,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{57C84C53-B905-437D-BEEF-7124C39AA062}">
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{57C84C53-B905-437D-BEEF-7124C39AA062}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,A1)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2329,10 +2418,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E11 A13:E17 A47:E51 A53:E57 A59:E63 A65:E69 A71:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A46:D46 A52:D52 A58:D58 A64:D64 A70:D70 G71:G1048576 A19:E34 A36:E45</xm:sqref>
+          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A52:E56 A58:E62 A64:E68 A70:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A57:D57 A63:D63 A69:D69 G70:G1048576 A48:E50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="endsWith" priority="17" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
+          <x14:cfRule type="endsWith" priority="20" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
             <xm:f>RIGHT(E4,LEN(Restrictions!$A$1))=Restrictions!$A$1</xm:f>
             <xm:f>Restrictions!$A$1</xm:f>
             <x14:dxf>
@@ -2343,7 +2432,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{CA908F4B-0D6A-49FA-81F5-C1AAB26EE444}">
+          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{CA908F4B-0D6A-49FA-81F5-C1AAB26EE444}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$C$1,E4)))</xm:f>
             <xm:f>Restrictions!$C$1</xm:f>
             <x14:dxf>
@@ -2354,7 +2443,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{BC07C843-4761-4226-B9B3-580ED2061AC2}">
+          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{BC07C843-4761-4226-B9B3-580ED2061AC2}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$D$1,E4)))</xm:f>
             <xm:f>Restrictions!$D$1</xm:f>
             <x14:dxf>
@@ -2365,10 +2454,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E11 E13:E17 E19:E34 E47:E51 E53:E57 E59:E63 E65:E69 E71:E1048576 E36:E45</xm:sqref>
+          <xm:sqref>E4:E11 E13:E17 E19:E34 E36:E46 E48:E50 E52:E56 E58:E62 E64:E68 E70:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F6)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2382,7 +2471,7 @@
           <xm:sqref>F6:F11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{7E01604B-B082-4DFB-908F-C0BF0EB6A591}">
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{7E01604B-B082-4DFB-908F-C0BF0EB6A591}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F13)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2396,7 +2485,7 @@
           <xm:sqref>F13:G17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{3FB18BD4-7343-4900-A7D7-1402CD6C7232}">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{3FB18BD4-7343-4900-A7D7-1402CD6C7232}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F19)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2410,7 +2499,7 @@
           <xm:sqref>F19:G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{756A584A-6AAC-4559-9F27-A59B4EFD7F34}">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{EACEB4CD-5C41-4F28-A4D3-D088DFF8444E}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F36)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2421,11 +2510,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F36:G45</xm:sqref>
+          <xm:sqref>F36:G46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{E988FD75-2909-4816-91C7-1018002A435D}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F47)))</xm:f>
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{E988FD75-2909-4816-91C7-1018002A435D}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F48)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2435,11 +2524,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F47:G51</xm:sqref>
+          <xm:sqref>F49:G49 F48 F50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{D5B6D5DF-9E2A-4C4B-BA82-97D983766AEE}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F53)))</xm:f>
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{D5B6D5DF-9E2A-4C4B-BA82-97D983766AEE}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F52)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2449,11 +2538,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F53:G57</xm:sqref>
+          <xm:sqref>F52:G56</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F59)))</xm:f>
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F58)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2463,11 +2552,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F59:G63</xm:sqref>
+          <xm:sqref>F58:G62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F65)))</xm:f>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F64)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2477,7 +2566,35 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F65:G69</xm:sqref>
+          <xm:sqref>F64:G68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{CEEE523A-4BD3-4918-8F98-4C43F3169196}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,G48)))</xm:f>
+            <xm:f>Restrictions!$B$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{69D9DE44-124B-4692-B922-EBD223C713CA}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,G50)))</xm:f>
+            <xm:f>Restrictions!$B$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G50</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2487,7 +2604,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E11 E13:E17 E71:E1048576 E19:E34 E47:E51 E53:E57 E59:E63 E65:E69 E36:E45</xm:sqref>
+          <xm:sqref>E1:E4 E6:E11 E13:E17 E70:E1048576 E19:E34 E48:E50 E52:E56 E58:E62 E64:E68 E36:E46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2503,7 +2620,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2525,6 +2642,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2767,27 +2904,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2804,29 +2946,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix(Enemies): Made skeletons not shoot on spawn
Skeletons can no longer shoot as soon as they spawn in
</commit_message>
<xml_diff>
--- a/T-P_POO-NeoDarbellay.xlsx
+++ b/T-P_POO-NeoDarbellay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\Vacances\P_POO-I320\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D97C530-466F-4051-A93F-47CEC88C1536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08C22AF-DA46-4678-BC03-30E4E85BE4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="0" windowWidth="21960" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="105">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -347,6 +347,27 @@
   </si>
   <si>
     <t>Took a 30 minute break in between to go eat</t>
+  </si>
+  <si>
+    <t>Downloading VS and Github Desktop again</t>
+  </si>
+  <si>
+    <t>The class computers got changed</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>Implementation of Issue #9 to the program</t>
+  </si>
+  <si>
+    <t>Fixed small issues and tweaked with some variables</t>
+  </si>
+  <si>
+    <t>Implementation of the base terrain</t>
+  </si>
+  <si>
+    <t>30m+, started again 13:10</t>
   </si>
 </sst>
 </file>
@@ -671,6 +692,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -683,30 +710,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -715,29 +718,33 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1134,89 +1141,89 @@
   </sheetPr>
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
+      <selection pane="bottomRight" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="50.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="36" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="32" t="s">
+      <c r="E1" s="40"/>
+      <c r="F1" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="33"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="34" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="32" t="s">
+      <c r="E2" s="40"/>
+      <c r="F2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="33"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="34" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="37"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="37"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1245,7 +1252,7 @@
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="29">
         <v>45929</v>
       </c>
       <c r="C6" s="5">
@@ -1262,11 +1269,11 @@
       </c>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="7">
         <v>20</v>
       </c>
@@ -1287,7 +1294,7 @@
       <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="7">
         <v>10</v>
       </c>
@@ -1306,7 +1313,7 @@
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="7">
         <v>35</v>
       </c>
@@ -1325,7 +1332,7 @@
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="7">
         <v>15</v>
       </c>
@@ -1346,7 +1353,7 @@
       <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="28"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="7">
         <v>35</v>
       </c>
@@ -1371,19 +1378,19 @@
       <c r="C12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="32">
         <f>SUM(C6:C11)</f>
         <v>140</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="29">
         <v>45930</v>
       </c>
       <c r="C13" s="5">
@@ -1406,7 +1413,7 @@
       <c r="A14" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="26">
         <v>10</v>
       </c>
@@ -1425,7 +1432,7 @@
       <c r="A15" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="26">
         <v>95</v>
       </c>
@@ -1444,7 +1451,7 @@
       <c r="A16" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="26">
         <v>15</v>
       </c>
@@ -1463,7 +1470,7 @@
       <c r="A17" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="26">
         <v>105</v>
       </c>
@@ -1490,19 +1497,19 @@
       <c r="C18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="32">
         <f>SUM(C13:C17)</f>
         <v>235</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="29">
         <v>45936</v>
       </c>
       <c r="C19" s="5">
@@ -1523,7 +1530,7 @@
       <c r="A20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="28"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="7">
         <v>20</v>
       </c>
@@ -1542,7 +1549,7 @@
       <c r="A21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="28"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="7">
         <v>15</v>
       </c>
@@ -1563,7 +1570,7 @@
       <c r="A22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="28"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="7">
         <v>10</v>
       </c>
@@ -1582,7 +1589,7 @@
       <c r="A23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="28"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="7">
         <v>10</v>
       </c>
@@ -1601,7 +1608,7 @@
       <c r="A24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="28"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="7">
         <v>25</v>
       </c>
@@ -1620,7 +1627,7 @@
       <c r="A25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="28"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="7">
         <v>15</v>
       </c>
@@ -1639,7 +1646,7 @@
       <c r="A26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="7">
         <v>20</v>
       </c>
@@ -1658,7 +1665,7 @@
       <c r="A27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="28"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="7">
         <v>5</v>
       </c>
@@ -1677,7 +1684,7 @@
       <c r="A28" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="28"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="7">
         <v>5</v>
       </c>
@@ -1696,7 +1703,7 @@
       <c r="A29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="28"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="7">
         <v>5</v>
       </c>
@@ -1715,7 +1722,7 @@
       <c r="A30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="28"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="7">
         <v>10</v>
       </c>
@@ -1734,7 +1741,7 @@
       <c r="A31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="28"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="7">
         <v>5</v>
       </c>
@@ -1753,7 +1760,7 @@
       <c r="A32" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="28"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="7">
         <v>15</v>
       </c>
@@ -1774,7 +1781,7 @@
       <c r="A33" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="28"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="7">
         <v>5</v>
       </c>
@@ -1793,7 +1800,7 @@
       <c r="A34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="28"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="7">
         <v>10</v>
       </c>
@@ -1820,19 +1827,19 @@
       <c r="C35" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D35" s="32">
         <f>SUM(C19:C34)</f>
         <v>185</v>
       </c>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B36" s="29">
         <v>45937</v>
       </c>
       <c r="C36" s="5">
@@ -1853,7 +1860,7 @@
       <c r="A37" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="28"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="26">
         <v>5</v>
       </c>
@@ -1872,7 +1879,7 @@
       <c r="A38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="28"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="26">
         <v>5</v>
       </c>
@@ -1891,7 +1898,7 @@
       <c r="A39" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="28"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="26">
         <v>5</v>
       </c>
@@ -1910,7 +1917,7 @@
       <c r="A40" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="28"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="26">
         <v>10</v>
       </c>
@@ -1929,7 +1936,7 @@
       <c r="A41" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="28"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="26">
         <v>140</v>
       </c>
@@ -1948,7 +1955,7 @@
       <c r="A42" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="28"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="26">
         <v>10</v>
       </c>
@@ -1967,7 +1974,7 @@
       <c r="A43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="28"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="26">
         <v>15</v>
       </c>
@@ -1986,7 +1993,7 @@
       <c r="A44" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="28"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="26">
         <v>10</v>
       </c>
@@ -2007,7 +2014,7 @@
       <c r="A45" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="28"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="26">
         <v>25</v>
       </c>
@@ -2028,7 +2035,7 @@
       <c r="A46" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="29"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="26">
         <v>5</v>
       </c>
@@ -2053,19 +2060,19 @@
       <c r="C47" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="38">
+      <c r="D47" s="32">
         <f>SUM(C36:C45)</f>
         <v>235</v>
       </c>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="39"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="33"/>
     </row>
     <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="27">
+      <c r="B48" s="29">
         <v>45954</v>
       </c>
       <c r="C48" s="5">
@@ -2088,7 +2095,7 @@
       <c r="A49" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="28"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="7">
         <v>85</v>
       </c>
@@ -2107,7 +2114,7 @@
       <c r="A50" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="28"/>
+      <c r="B50" s="30"/>
       <c r="C50" s="7">
         <v>170</v>
       </c>
@@ -2134,53 +2141,91 @@
       <c r="C51" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="38">
+      <c r="D51" s="32">
         <f>SUM(C48:C50)</f>
         <v>325</v>
       </c>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="39"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="33"/>
     </row>
     <row r="52" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="19"/>
-    </row>
-    <row r="53" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="22"/>
+      <c r="A52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="29">
+        <v>45957</v>
+      </c>
+      <c r="C52" s="5">
+        <v>20</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="30"/>
+      <c r="C53" s="7">
+        <v>50</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F53" s="23">
+        <v>0.49305555555555558</v>
+      </c>
       <c r="G53" s="19"/>
     </row>
     <row r="54" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="28"/>
+      <c r="A54" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="30"/>
       <c r="C54" s="7"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="D54" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F54" s="7"/>
-      <c r="G54" s="19"/>
+      <c r="G54" s="19" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="28"/>
+      <c r="A55" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="30"/>
       <c r="C55" s="7"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="D55" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="F55" s="7"/>
       <c r="G55" s="19"/>
     </row>
     <row r="56" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
-      <c r="B56" s="29"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="9"/>
       <c r="D56" s="8"/>
       <c r="E56" s="10"/>
@@ -2197,17 +2242,17 @@
       <c r="C57" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="38">
+      <c r="D57" s="32">
         <f>SUM(C52:C56)</f>
-        <v>0</v>
-      </c>
-      <c r="E57" s="38"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="39"/>
+        <v>70</v>
+      </c>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="33"/>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="27"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="5"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
@@ -2216,7 +2261,7 @@
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
-      <c r="B59" s="28"/>
+      <c r="B59" s="30"/>
       <c r="C59" s="7"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
@@ -2225,7 +2270,7 @@
     </row>
     <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
-      <c r="B60" s="28"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="7"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
@@ -2234,7 +2279,7 @@
     </row>
     <row r="61" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
-      <c r="B61" s="28"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="7"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
@@ -2243,7 +2288,7 @@
     </row>
     <row r="62" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
-      <c r="B62" s="29"/>
+      <c r="B62" s="31"/>
       <c r="C62" s="9"/>
       <c r="D62" s="8"/>
       <c r="E62" s="10"/>
@@ -2260,17 +2305,17 @@
       <c r="C63" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="38">
+      <c r="D63" s="32">
         <f>SUM(C58:C62)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="39"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="33"/>
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
-      <c r="B64" s="27"/>
+      <c r="B64" s="29"/>
       <c r="C64" s="5"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
@@ -2279,7 +2324,7 @@
     </row>
     <row r="65" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
-      <c r="B65" s="28"/>
+      <c r="B65" s="30"/>
       <c r="C65" s="7"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
@@ -2288,7 +2333,7 @@
     </row>
     <row r="66" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
-      <c r="B66" s="28"/>
+      <c r="B66" s="30"/>
       <c r="C66" s="7"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
@@ -2297,7 +2342,7 @@
     </row>
     <row r="67" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
-      <c r="B67" s="28"/>
+      <c r="B67" s="30"/>
       <c r="C67" s="7"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
@@ -2306,7 +2351,7 @@
     </row>
     <row r="68" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="9"/>
-      <c r="B68" s="29"/>
+      <c r="B68" s="31"/>
       <c r="C68" s="9"/>
       <c r="D68" s="8"/>
       <c r="E68" s="10"/>
@@ -2323,22 +2368,22 @@
       <c r="C69" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D69" s="38">
+      <c r="D69" s="32">
         <f>SUM(C64:C68)</f>
         <v>0</v>
       </c>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="39"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="33"/>
     </row>
     <row r="70" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="30" t="s">
+      <c r="A70" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B70" s="31"/>
+      <c r="B70" s="28"/>
       <c r="C70" s="12">
         <f>MROUND(SUM(C6:C69) /60,0.2)</f>
-        <v>18.8</v>
+        <v>20</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="18"/>
@@ -2355,13 +2400,9 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="B19:B34"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="D63:G63"/>
-    <mergeCell ref="B36:B46"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B13:B17"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -2371,17 +2412,21 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="B64:B68"/>
     <mergeCell ref="D12:G12"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="B19:B34"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="B36:B46"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="B52:B56"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="B64:B68"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
@@ -2407,7 +2452,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{57C84C53-B905-437D-BEEF-7124C39AA062}">
+          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{57C84C53-B905-437D-BEEF-7124C39AA062}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,A1)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2418,10 +2463,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A52:E56 A58:E62 A64:E68 A70:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A57:D57 A63:D63 A69:D69 G70:G1048576 A48:E50</xm:sqref>
+          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A58:E62 A64:E68 A70:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A57:D57 A63:D63 A69:D69 G70:G1048576 A52:E56</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="endsWith" priority="20" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
+          <x14:cfRule type="endsWith" priority="21" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
             <xm:f>RIGHT(E4,LEN(Restrictions!$A$1))=Restrictions!$A$1</xm:f>
             <xm:f>Restrictions!$A$1</xm:f>
             <x14:dxf>
@@ -2432,7 +2477,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{CA908F4B-0D6A-49FA-81F5-C1AAB26EE444}">
+          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{CA908F4B-0D6A-49FA-81F5-C1AAB26EE444}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$C$1,E4)))</xm:f>
             <xm:f>Restrictions!$C$1</xm:f>
             <x14:dxf>
@@ -2443,7 +2488,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{BC07C843-4761-4226-B9B3-580ED2061AC2}">
+          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{BC07C843-4761-4226-B9B3-580ED2061AC2}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$D$1,E4)))</xm:f>
             <xm:f>Restrictions!$D$1</xm:f>
             <x14:dxf>
@@ -2457,7 +2502,7 @@
           <xm:sqref>E4:E11 E13:E17 E19:E34 E36:E46 E48:E50 E52:E56 E58:E62 E64:E68 E70:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
+          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F6)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2471,7 +2516,7 @@
           <xm:sqref>F6:F11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{7E01604B-B082-4DFB-908F-C0BF0EB6A591}">
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{7E01604B-B082-4DFB-908F-C0BF0EB6A591}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F13)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2485,7 +2530,7 @@
           <xm:sqref>F13:G17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{3FB18BD4-7343-4900-A7D7-1402CD6C7232}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{3FB18BD4-7343-4900-A7D7-1402CD6C7232}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F19)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2499,7 +2544,7 @@
           <xm:sqref>F19:G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{EACEB4CD-5C41-4F28-A4D3-D088DFF8444E}">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{EACEB4CD-5C41-4F28-A4D3-D088DFF8444E}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F36)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2513,7 +2558,7 @@
           <xm:sqref>F36:G46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{E988FD75-2909-4816-91C7-1018002A435D}">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{69D9DE44-124B-4692-B922-EBD223C713CA}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F48)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2524,10 +2569,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F49:G49 F48 F50</xm:sqref>
+          <xm:sqref>F48:G50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{D5B6D5DF-9E2A-4C4B-BA82-97D983766AEE}">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{53DAE65F-9801-42EC-8B5C-059A8A03D0AB}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F52)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2541,7 +2586,7 @@
           <xm:sqref>F52:G56</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F58)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2555,7 +2600,7 @@
           <xm:sqref>F58:G62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F64)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2567,34 +2612,6 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>F64:G68</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{CEEE523A-4BD3-4918-8F98-4C43F3169196}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,G48)))</xm:f>
-            <xm:f>Restrictions!$B$1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF00B0F0"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G48</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{69D9DE44-124B-4692-B922-EBD223C713CA}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,G50)))</xm:f>
-            <xm:f>Restrictions!$B$1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF00B0F0"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G50</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2620,7 +2637,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
feat(Main): Added a map to the game
</commit_message>
<xml_diff>
--- a/T-P_POO-NeoDarbellay.xlsx
+++ b/T-P_POO-NeoDarbellay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08C22AF-DA46-4678-BC03-30E4E85BE4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922EEC93-FE63-459F-8F00-6E10074D4EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Restrictions" sheetId="19" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$70</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$68</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="104">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -365,9 +365,6 @@
   </si>
   <si>
     <t>Implementation of the base terrain</t>
-  </si>
-  <si>
-    <t>30m+, started again 13:10</t>
   </si>
 </sst>
 </file>
@@ -1139,13 +1136,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F54" sqref="F54"/>
+      <selection pane="bottomRight" activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2191,72 +2188,72 @@
       </c>
       <c r="G53" s="19"/>
     </row>
-    <row r="54" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B54" s="30"/>
-      <c r="C54" s="7"/>
+      <c r="C54" s="7">
+        <v>125</v>
+      </c>
       <c r="D54" s="8" t="s">
         <v>103</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F54" s="23">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="G54" s="19"/>
+    </row>
+    <row r="55" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="32">
+        <f>SUM(C52:C54)</f>
+        <v>195</v>
+      </c>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="33"/>
+    </row>
+    <row r="56" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="19"/>
-    </row>
-    <row r="56" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="7"/>
+      <c r="F56" s="22"/>
       <c r="G56" s="19"/>
     </row>
-    <row r="57" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" s="32">
-        <f>SUM(C52:C56)</f>
-        <v>70</v>
-      </c>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="33"/>
+    <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="5"/>
+      <c r="A58" s="6"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="7"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
-      <c r="F58" s="22"/>
+      <c r="F58" s="7"/>
       <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2265,61 +2262,61 @@
       <c r="C59" s="7"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
-      <c r="F59" s="22"/>
+      <c r="F59" s="7"/>
       <c r="G59" s="19"/>
     </row>
-    <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="7"/>
+    <row r="60" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="9"/>
       <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+      <c r="E60" s="10"/>
       <c r="F60" s="7"/>
       <c r="G60" s="19"/>
     </row>
-    <row r="61" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="19"/>
-    </row>
-    <row r="62" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="9"/>
+    <row r="61" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="32">
+        <f>SUM(C56:C60)</f>
+        <v>0</v>
+      </c>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="33"/>
+    </row>
+    <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="5"/>
       <c r="D62" s="8"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="7"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="22"/>
       <c r="G62" s="19"/>
     </row>
-    <row r="63" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="32">
-        <f>SUM(C58:C62)</f>
-        <v>0</v>
-      </c>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="33"/>
+    <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="19"/>
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="29"/>
-      <c r="C64" s="5"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="7"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
-      <c r="F64" s="22"/>
+      <c r="F64" s="7"/>
       <c r="G64" s="19"/>
     </row>
     <row r="65" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2328,75 +2325,57 @@
       <c r="C65" s="7"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
-      <c r="F65" s="22"/>
+      <c r="F65" s="7"/>
       <c r="G65" s="19"/>
     </row>
-    <row r="66" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="7"/>
+    <row r="66" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="9"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="9"/>
       <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
+      <c r="E66" s="10"/>
       <c r="F66" s="7"/>
       <c r="G66" s="19"/>
     </row>
-    <row r="67" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="19"/>
-    </row>
-    <row r="68" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="19"/>
-    </row>
-    <row r="69" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
+    <row r="67" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B67" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="C67" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D69" s="32">
-        <f>SUM(C64:C68)</f>
+      <c r="D67" s="32">
+        <f>SUM(C62:C66)</f>
         <v>0</v>
       </c>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="33"/>
-    </row>
-    <row r="70" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="27" t="s">
+      <c r="E67" s="32"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="33"/>
+    </row>
+    <row r="68" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B70" s="28"/>
-      <c r="C70" s="12">
-        <f>MROUND(SUM(C6:C69) /60,0.2)</f>
-        <v>20</v>
-      </c>
-      <c r="D70" s="13"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="14"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="B68" s="28"/>
+      <c r="C68" s="12">
+        <f>MROUND(SUM(C6:C67) /60,0.2)</f>
+        <v>22</v>
+      </c>
+      <c r="D68" s="13"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="14"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="27">
@@ -2412,28 +2391,28 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B62:B66"/>
     <mergeCell ref="D12:G12"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="D67:G67"/>
     <mergeCell ref="B19:B34"/>
     <mergeCell ref="D47:G47"/>
     <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D61:G61"/>
     <mergeCell ref="B36:B46"/>
     <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B52:B54"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C64:C68 C52:C56 C58:C62 C6:C11 B6 C13:C17 C19:C34 C48:C50 C36:C46" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C62:C66 C52:C54 C56:C60 C6:C11 B6 C13:C17 C19:C34 C48:C50 C36:C46" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B13:B17 B64:B68 B19:B34 B48:B50 B52:B56 B58:B62 B36" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B13:B17 B62:B66 B19:B34 B48:B50 B52:B54 B56:B60 B36" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -2463,7 +2442,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A58:E62 A64:E68 A70:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A57:D57 A63:D63 A69:D69 G70:G1048576 A52:E56</xm:sqref>
+          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A62:E66 A68:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A55:D55 A61:D61 A67:D67 G68:G1048576 A52:E54 A56:E60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="21" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
@@ -2499,7 +2478,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E11 E13:E17 E19:E34 E36:E46 E48:E50 E52:E56 E58:E62 E64:E68 E70:E1048576</xm:sqref>
+          <xm:sqref>E4:E11 E13:E17 E19:E34 E36:E46 E48:E50 E52:E54 E56:E60 E62:E66 E68:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="18" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
@@ -2583,11 +2562,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F52:G56</xm:sqref>
+          <xm:sqref>F52:G54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="12" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F58)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F56)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2597,11 +2576,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F58:G62</xm:sqref>
+          <xm:sqref>F56:G60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="11" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F64)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F62)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2611,7 +2590,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F64:G68</xm:sqref>
+          <xm:sqref>F62:G66</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2621,7 +2600,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E11 E13:E17 E70:E1048576 E19:E34 E48:E50 E52:E56 E58:E62 E64:E68 E36:E46</xm:sqref>
+          <xm:sqref>E1:E4 E6:E11 E13:E17 E68:E1048576 E19:E34 E48:E50 E52:E54 E56:E60 E62:E66 E36:E46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
feat(main): Implemented the score system
</commit_message>
<xml_diff>
--- a/T-P_POO-NeoDarbellay.xlsx
+++ b/T-P_POO-NeoDarbellay.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922EEC93-FE63-459F-8F00-6E10074D4EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B6DC56-8931-42A8-97B6-3E4FEFE9660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="104">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -689,11 +689,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -703,6 +706,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -714,27 +735,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1139,10 +1139,10 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E56" sqref="E56"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56:B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1162,65 +1162,65 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="39" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="37" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="38"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="39" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="37" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="38"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="39" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="34" t="s">
+      <c r="E3" s="35"/>
+      <c r="F3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1249,7 +1249,7 @@
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="30">
         <v>45929</v>
       </c>
       <c r="C6" s="5">
@@ -1270,7 +1270,7 @@
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="30"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="7">
         <v>20</v>
       </c>
@@ -1291,7 +1291,7 @@
       <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="7">
         <v>10</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="30"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="7">
         <v>35</v>
       </c>
@@ -1329,7 +1329,7 @@
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="7">
         <v>15</v>
       </c>
@@ -1350,7 +1350,7 @@
       <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="30"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="7">
         <v>35</v>
       </c>
@@ -1375,19 +1375,19 @@
       <c r="C12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="39">
         <f>SUM(C6:C11)</f>
         <v>140</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="30">
         <v>45930</v>
       </c>
       <c r="C13" s="5">
@@ -1410,7 +1410,7 @@
       <c r="A14" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="26">
         <v>10</v>
       </c>
@@ -1429,7 +1429,7 @@
       <c r="A15" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="30"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="26">
         <v>95</v>
       </c>
@@ -1448,7 +1448,7 @@
       <c r="A16" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="26">
         <v>15</v>
       </c>
@@ -1467,7 +1467,7 @@
       <c r="A17" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="30"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="26">
         <v>105</v>
       </c>
@@ -1494,19 +1494,19 @@
       <c r="C18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="39">
         <f>SUM(C13:C17)</f>
         <v>235</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
     </row>
     <row r="19" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="30">
         <v>45936</v>
       </c>
       <c r="C19" s="5">
@@ -1527,7 +1527,7 @@
       <c r="A20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="30"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="7">
         <v>20</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="A21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="30"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="7">
         <v>15</v>
       </c>
@@ -1567,7 +1567,7 @@
       <c r="A22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="30"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="7">
         <v>10</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="A23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="30"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="7">
         <v>10</v>
       </c>
@@ -1605,7 +1605,7 @@
       <c r="A24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="30"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="7">
         <v>25</v>
       </c>
@@ -1624,7 +1624,7 @@
       <c r="A25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="30"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="7">
         <v>15</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="A26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="30"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="7">
         <v>20</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="A27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="30"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="7">
         <v>5</v>
       </c>
@@ -1681,7 +1681,7 @@
       <c r="A28" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="30"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="7">
         <v>5</v>
       </c>
@@ -1700,7 +1700,7 @@
       <c r="A29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="30"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="7">
         <v>5</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="A30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="30"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="7">
         <v>10</v>
       </c>
@@ -1738,7 +1738,7 @@
       <c r="A31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="30"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="7">
         <v>5</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="A32" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="30"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="7">
         <v>15</v>
       </c>
@@ -1778,7 +1778,7 @@
       <c r="A33" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="30"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="7">
         <v>5</v>
       </c>
@@ -1797,7 +1797,7 @@
       <c r="A34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="30"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="7">
         <v>10</v>
       </c>
@@ -1824,19 +1824,19 @@
       <c r="C35" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="32">
+      <c r="D35" s="39">
         <f>SUM(C19:C34)</f>
         <v>185</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="29">
+      <c r="B36" s="30">
         <v>45937</v>
       </c>
       <c r="C36" s="5">
@@ -1857,7 +1857,7 @@
       <c r="A37" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="30"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="26">
         <v>5</v>
       </c>
@@ -1876,7 +1876,7 @@
       <c r="A38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="30"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="26">
         <v>5</v>
       </c>
@@ -1895,7 +1895,7 @@
       <c r="A39" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="30"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="26">
         <v>5</v>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="A40" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="30"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="26">
         <v>10</v>
       </c>
@@ -1933,7 +1933,7 @@
       <c r="A41" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="30"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="26">
         <v>140</v>
       </c>
@@ -1952,7 +1952,7 @@
       <c r="A42" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="26">
         <v>10</v>
       </c>
@@ -1971,7 +1971,7 @@
       <c r="A43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="26">
         <v>15</v>
       </c>
@@ -1990,7 +1990,7 @@
       <c r="A44" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="30"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="26">
         <v>10</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="A45" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="30"/>
+      <c r="B45" s="31"/>
       <c r="C45" s="26">
         <v>25</v>
       </c>
@@ -2032,7 +2032,7 @@
       <c r="A46" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="31"/>
+      <c r="B46" s="38"/>
       <c r="C46" s="26">
         <v>5</v>
       </c>
@@ -2057,19 +2057,19 @@
       <c r="C47" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="32">
+      <c r="D47" s="39">
         <f>SUM(C36:C45)</f>
         <v>235</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="33"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="40"/>
     </row>
     <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="29">
+      <c r="B48" s="30">
         <v>45954</v>
       </c>
       <c r="C48" s="5">
@@ -2092,7 +2092,7 @@
       <c r="A49" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="30"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="7">
         <v>85</v>
       </c>
@@ -2111,7 +2111,7 @@
       <c r="A50" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="30"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="7">
         <v>170</v>
       </c>
@@ -2138,19 +2138,19 @@
       <c r="C51" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="32">
+      <c r="D51" s="39">
         <f>SUM(C48:C50)</f>
         <v>325</v>
       </c>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="33"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="40"/>
     </row>
     <row r="52" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="29">
+      <c r="B52" s="30">
         <v>45957</v>
       </c>
       <c r="C52" s="5">
@@ -2173,7 +2173,7 @@
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="30"/>
+      <c r="B53" s="31"/>
       <c r="C53" s="7">
         <v>50</v>
       </c>
@@ -2192,7 +2192,7 @@
       <c r="A54" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="30"/>
+      <c r="B54" s="31"/>
       <c r="C54" s="7">
         <v>125</v>
       </c>
@@ -2217,30 +2217,38 @@
       <c r="C55" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D55" s="32">
+      <c r="D55" s="39">
         <f>SUM(C52:C54)</f>
         <v>195</v>
       </c>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="33"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="40"/>
     </row>
     <row r="56" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="5"/>
+      <c r="A56" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="30">
+        <v>45958</v>
+      </c>
+      <c r="C56" s="5">
+        <v>25</v>
+      </c>
       <c r="D56" s="8" t="s">
         <v>101</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F56" s="22"/>
+        <v>32</v>
+      </c>
+      <c r="F56" s="23">
+        <v>0.56597222222222221</v>
+      </c>
       <c r="G56" s="19"/>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
-      <c r="B57" s="30"/>
+      <c r="B57" s="31"/>
       <c r="C57" s="7"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
@@ -2249,7 +2257,7 @@
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
-      <c r="B58" s="30"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="7"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
@@ -2258,7 +2266,7 @@
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
-      <c r="B59" s="30"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="7"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
@@ -2267,7 +2275,7 @@
     </row>
     <row r="60" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
-      <c r="B60" s="31"/>
+      <c r="B60" s="38"/>
       <c r="C60" s="9"/>
       <c r="D60" s="8"/>
       <c r="E60" s="10"/>
@@ -2284,17 +2292,17 @@
       <c r="C61" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D61" s="32">
+      <c r="D61" s="39">
         <f>SUM(C56:C60)</f>
-        <v>0</v>
-      </c>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="33"/>
+        <v>25</v>
+      </c>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="40"/>
     </row>
     <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
-      <c r="B62" s="29"/>
+      <c r="B62" s="30"/>
       <c r="C62" s="5"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
@@ -2303,7 +2311,7 @@
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
-      <c r="B63" s="30"/>
+      <c r="B63" s="31"/>
       <c r="C63" s="7"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
@@ -2312,7 +2320,7 @@
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
-      <c r="B64" s="30"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="7"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
@@ -2321,7 +2329,7 @@
     </row>
     <row r="65" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
-      <c r="B65" s="30"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="7"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
@@ -2330,7 +2338,7 @@
     </row>
     <row r="66" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
-      <c r="B66" s="31"/>
+      <c r="B66" s="38"/>
       <c r="C66" s="9"/>
       <c r="D66" s="8"/>
       <c r="E66" s="10"/>
@@ -2347,22 +2355,22 @@
       <c r="C67" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="32">
+      <c r="D67" s="39">
         <f>SUM(C62:C66)</f>
         <v>0</v>
       </c>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="33"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="40"/>
     </row>
     <row r="68" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="27" t="s">
+      <c r="A68" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B68" s="28"/>
+      <c r="B68" s="37"/>
       <c r="C68" s="12">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>22</v>
+        <v>22.400000000000002</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="18"/>
@@ -2379,18 +2387,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B62:B66"/>
@@ -2406,6 +2402,18 @@
     <mergeCell ref="B36:B46"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
@@ -2442,7 +2450,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A62:E66 A68:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A55:D55 A61:D61 A67:D67 G68:G1048576 A52:E54 A56:E60</xm:sqref>
+          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A52:E54 A56:E60 A62:E66 A68:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A55:D55 A61:D61 A67:D67 G68:G1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="21" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
@@ -2638,26 +2646,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2900,32 +2888,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2942,4 +2925,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore(main): Simplified the class constructors
I also implemented new constructors
</commit_message>
<xml_diff>
--- a/T-P_POO-NeoDarbellay.xlsx
+++ b/T-P_POO-NeoDarbellay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B6DC56-8931-42A8-97B6-3E4FEFE9660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F80540-3E2C-4F24-9CAD-A592121ECC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>Implementation of the base terrain</t>
+  </si>
+  <si>
+    <t>Changed the constructors of multiple classes so that Object creation is easier</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1145,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B56" sqref="B56:B60"/>
+      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2246,13 +2249,23 @@
       </c>
       <c r="G56" s="19"/>
     </row>
-    <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
+    <row r="57" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B57" s="31"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="22"/>
+      <c r="C57" s="7">
+        <v>20</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F57" s="23">
+        <v>0.57986111111111105</v>
+      </c>
       <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2294,7 +2307,7 @@
       </c>
       <c r="D61" s="39">
         <f>SUM(C56:C60)</f>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E61" s="39"/>
       <c r="F61" s="39"/>
@@ -2370,7 +2383,7 @@
       <c r="B68" s="37"/>
       <c r="C68" s="12">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>22.400000000000002</v>
+        <v>22.8</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="18"/>

</xml_diff>

<commit_message>
feat(Main): Added a title screen
Along with that, i moved MoveEnemy() to Enemy.cs and renamed it Move()
</commit_message>
<xml_diff>
--- a/T-P_POO-NeoDarbellay.xlsx
+++ b/T-P_POO-NeoDarbellay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F80540-3E2C-4F24-9CAD-A592121ECC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4986095A-F5EC-4B1C-955C-C2BC691EE4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="106">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>Changed the constructors of multiple classes so that Object creation is easier</t>
+  </si>
+  <si>
+    <t>Implementation of Issue #10 to the program</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1148,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomRight" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2269,12 +2272,22 @@
       <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
+      <c r="A58" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B58" s="31"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="7"/>
+      <c r="C58" s="7">
+        <v>50</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" s="23">
+        <v>0.61458333333333337</v>
+      </c>
       <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2307,7 +2320,7 @@
       </c>
       <c r="D61" s="39">
         <f>SUM(C56:C60)</f>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="E61" s="39"/>
       <c r="F61" s="39"/>
@@ -2383,7 +2396,7 @@
       <c r="B68" s="37"/>
       <c r="C68" s="12">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>22.8</v>
+        <v>23.6</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="18"/>

</xml_diff>

<commit_message>
feat(main): Implemented Issue #7
I forgot to mention, but Issue #10  and #9 have been implemented in the previous commits of today
</commit_message>
<xml_diff>
--- a/T-P_POO-NeoDarbellay.xlsx
+++ b/T-P_POO-NeoDarbellay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4986095A-F5EC-4B1C-955C-C2BC691EE4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F843FB39-7BD7-4C86-98E8-7696990BB991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Restrictions" sheetId="19" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$70</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -371,6 +371,15 @@
   </si>
   <si>
     <t>Implementation of Issue #10 to the program</t>
+  </si>
+  <si>
+    <t>Implementation of Issue #7 to the program</t>
+  </si>
+  <si>
+    <t>Creation of new enemy types for issue #7</t>
+  </si>
+  <si>
+    <t>Fixed small issues with map position</t>
   </si>
 </sst>
 </file>
@@ -1142,13 +1151,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2283,7 +2292,7 @@
         <v>105</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F58" s="23">
         <v>0.61458333333333337</v>
@@ -2291,66 +2300,96 @@
       <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
+      <c r="A59" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="B59" s="31"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="7"/>
+      <c r="C59" s="7">
+        <v>30</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F59" s="23">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G59" s="19"/>
     </row>
-    <row r="60" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="7"/>
+    <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" s="31"/>
+      <c r="C60" s="9">
+        <v>30</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="23">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="G60" s="19"/>
     </row>
-    <row r="61" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="11" t="s">
+    <row r="61" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="31"/>
+      <c r="C61" s="9">
+        <v>35</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" s="23">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="G61" s="19"/>
+    </row>
+    <row r="62" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="6"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="19"/>
+    </row>
+    <row r="63" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B63" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C63" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D61" s="39">
-        <f>SUM(C56:C60)</f>
-        <v>95</v>
-      </c>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="40"/>
-    </row>
-    <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="19"/>
-    </row>
-    <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="19"/>
+      <c r="D63" s="39">
+        <f>SUM(C56:C62)</f>
+        <v>190</v>
+      </c>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="40"/>
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="7"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="5"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
-      <c r="F64" s="7"/>
+      <c r="F64" s="22"/>
       <c r="G64" s="19"/>
     </row>
     <row r="65" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2359,72 +2398,90 @@
       <c r="C65" s="7"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
-      <c r="F65" s="7"/>
+      <c r="F65" s="22"/>
       <c r="G65" s="19"/>
     </row>
-    <row r="66" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
-      <c r="B66" s="38"/>
-      <c r="C66" s="9"/>
+    <row r="66" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="7"/>
       <c r="D66" s="8"/>
-      <c r="E66" s="10"/>
+      <c r="E66" s="8"/>
       <c r="F66" s="7"/>
       <c r="G66" s="19"/>
     </row>
-    <row r="67" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="11" t="s">
+    <row r="67" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="19"/>
+    </row>
+    <row r="68" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="9"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="19"/>
+    </row>
+    <row r="69" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B69" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="C69" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="39">
-        <f>SUM(C62:C66)</f>
+      <c r="D69" s="39">
+        <f>SUM(C64:C68)</f>
         <v>0</v>
       </c>
-      <c r="E67" s="39"/>
-      <c r="F67" s="39"/>
-      <c r="G67" s="40"/>
-    </row>
-    <row r="68" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="36" t="s">
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="40"/>
+    </row>
+    <row r="70" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B68" s="37"/>
-      <c r="C68" s="12">
-        <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>23.6</v>
-      </c>
-      <c r="D68" s="13"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="14"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+      <c r="B70" s="37"/>
+      <c r="C70" s="12">
+        <f>MROUND(SUM(C6:C69) /60,0.2)</f>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="D70" s="13"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="14"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="B56:B62"/>
+    <mergeCell ref="B64:B68"/>
     <mergeCell ref="D12:G12"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="D69:G69"/>
     <mergeCell ref="B19:B34"/>
     <mergeCell ref="D47:G47"/>
     <mergeCell ref="D51:G51"/>
     <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D63:G63"/>
     <mergeCell ref="B36:B46"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="B52:B54"/>
@@ -2443,10 +2500,10 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C62:C66 C52:C54 C56:C60 C6:C11 B6 C13:C17 C19:C34 C48:C50 C36:C46" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C64:C68 C52:C54 C36:C46 C6:C11 B6 C13:C17 C19:C34 C48:C50 C56:C62" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B13:B17 B62:B66 B19:B34 B48:B50 B52:B54 B56:B60 B36" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B13:B17 B64:B68 B19:B34 B48:B50 B52:B54 B36 B56:B62" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -2476,7 +2533,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A52:E54 A56:E60 A62:E66 A68:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A55:D55 A61:D61 A67:D67 G68:G1048576</xm:sqref>
+          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A52:E54 A64:E68 A70:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A55:D55 A63:D63 A69:D69 G70:G1048576 A56:E62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="21" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
@@ -2512,7 +2569,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E11 E13:E17 E19:E34 E36:E46 E48:E50 E52:E54 E56:E60 E62:E66 E68:E1048576</xm:sqref>
+          <xm:sqref>E4:E11 E13:E17 E19:E34 E36:E46 E48:E50 E52:E54 E64:E68 E70:E1048576 E56:E62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="18" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
@@ -2610,11 +2667,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F56:G60</xm:sqref>
+          <xm:sqref>F56:G62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="11" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F62)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F64)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2624,7 +2681,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F62:G66</xm:sqref>
+          <xm:sqref>F64:G68</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2634,7 +2691,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E11 E13:E17 E68:E1048576 E19:E34 E48:E50 E52:E54 E56:E60 E62:E66 E36:E46</xm:sqref>
+          <xm:sqref>E1:E4 E6:E11 E13:E17 E70:E1048576 E19:E34 E48:E50 E52:E54 E36:E46 E64:E68 E56:E62</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
feat(main): Finished the project
</commit_message>
<xml_diff>
--- a/T-P_POO-NeoDarbellay.xlsx
+++ b/T-P_POO-NeoDarbellay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01Modules\02Deuxieme_Annee\Trimestre_1\I320\P_POO\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F843FB39-7BD7-4C86-98E8-7696990BB991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727CD5B9-C0AF-444B-9FC6-78293AD44435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Restrictions" sheetId="19" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$70</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$72</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="114">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -379,7 +379,22 @@
     <t>Creation of new enemy types for issue #7</t>
   </si>
   <si>
+    <t>Creation of more waves</t>
+  </si>
+  <si>
     <t>Fixed small issues with map position</t>
+  </si>
+  <si>
+    <t>Testing the game out</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Releasing the final version to GitHub</t>
+  </si>
+  <si>
+    <t>GitHub</t>
   </si>
 </sst>
 </file>
@@ -1151,13 +1166,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
+      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2327,7 +2342,7 @@
         <v>30</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E60" s="10" t="s">
         <v>32</v>
@@ -2356,58 +2371,88 @@
       </c>
       <c r="G61" s="19"/>
     </row>
-    <row r="62" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="6"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="7"/>
+    <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" s="31"/>
+      <c r="C62" s="9">
+        <v>25</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" s="23">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="G62" s="19"/>
     </row>
-    <row r="63" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
+    <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="31"/>
+      <c r="C63" s="9">
+        <v>5</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F63" s="23">
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="G63" s="19"/>
+    </row>
+    <row r="64" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" s="38"/>
+      <c r="C64" s="9">
+        <v>10</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64" s="23">
+        <v>0.71875</v>
+      </c>
+      <c r="G64" s="19"/>
+    </row>
+    <row r="65" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B65" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C65" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="39">
-        <f>SUM(C56:C62)</f>
-        <v>190</v>
-      </c>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="40"/>
-    </row>
-    <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="19"/>
-    </row>
-    <row r="65" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="19"/>
+      <c r="D65" s="39">
+        <f>SUM(C56:C64)</f>
+        <v>230</v>
+      </c>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="40"/>
     </row>
     <row r="66" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="7"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="5"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
-      <c r="F66" s="7"/>
+      <c r="F66" s="22"/>
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2416,72 +2461,90 @@
       <c r="C67" s="7"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
-      <c r="F67" s="7"/>
+      <c r="F67" s="22"/>
       <c r="G67" s="19"/>
     </row>
-    <row r="68" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
-      <c r="B68" s="38"/>
-      <c r="C68" s="9"/>
+    <row r="68" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="7"/>
       <c r="D68" s="8"/>
-      <c r="E68" s="10"/>
+      <c r="E68" s="8"/>
       <c r="F68" s="7"/>
       <c r="G68" s="19"/>
     </row>
-    <row r="69" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
+    <row r="69" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="19"/>
+    </row>
+    <row r="70" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="9"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="19"/>
+    </row>
+    <row r="71" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B71" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="C71" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D69" s="39">
-        <f>SUM(C64:C68)</f>
+      <c r="D71" s="39">
+        <f>SUM(C66:C70)</f>
         <v>0</v>
       </c>
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
-      <c r="G69" s="40"/>
-    </row>
-    <row r="70" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="36" t="s">
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="40"/>
+    </row>
+    <row r="72" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B70" s="37"/>
-      <c r="C70" s="12">
-        <f>MROUND(SUM(C6:C69) /60,0.2)</f>
-        <v>25.200000000000003</v>
-      </c>
-      <c r="D70" s="13"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="14"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="B72" s="37"/>
+      <c r="C72" s="12">
+        <f>MROUND(SUM(C6:C71) /60,0.2)</f>
+        <v>25.8</v>
+      </c>
+      <c r="D72" s="13"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="14"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B56:B62"/>
-    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="B56:B64"/>
+    <mergeCell ref="B66:B70"/>
     <mergeCell ref="D12:G12"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="D71:G71"/>
     <mergeCell ref="B19:B34"/>
     <mergeCell ref="D47:G47"/>
     <mergeCell ref="D51:G51"/>
     <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="D65:G65"/>
     <mergeCell ref="B36:B46"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="B52:B54"/>
@@ -2500,10 +2563,10 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C64:C68 C52:C54 C36:C46 C6:C11 B6 C13:C17 C19:C34 C48:C50 C56:C62" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C66:C70 C52:C54 C36:C46 C6:C11 B6 C13:C17 C19:C34 C48:C50 C56:C64" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B13:B17 B64:B68 B19:B34 B48:B50 B52:B54 B36 B56:B62" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B13:B17 B66:B70 B19:B34 B48:B50 B52:B54 B36 B56:B64" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -2533,7 +2596,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A52:E54 A64:E68 A70:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A55:D55 A63:D63 A69:D69 G70:G1048576 A56:E62</xm:sqref>
+          <xm:sqref>A4:E11 A13:E17 A19:E34 A36:E36 C37:E46 A48:E50 A52:E54 A66:E70 A72:E1048576 A1:D3 F1:F3 G4:G6 G8:G11 A12:D12 A18:D18 A35:D35 A37:A46 A47:D47 A51:D51 A55:D55 A65:D65 A71:D71 G72:G1048576 A56:E64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="21" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
@@ -2569,7 +2632,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E11 E13:E17 E19:E34 E36:E46 E48:E50 E52:E54 E64:E68 E70:E1048576 E56:E62</xm:sqref>
+          <xm:sqref>E4:E11 E13:E17 E19:E34 E36:E46 E48:E50 E52:E54 E66:E70 E72:E1048576 E56:E64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="18" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
@@ -2667,11 +2730,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F56:G62</xm:sqref>
+          <xm:sqref>F56:G64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="11" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F64)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F66)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -2681,7 +2744,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F64:G68</xm:sqref>
+          <xm:sqref>F66:G70</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2691,7 +2754,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E11 E13:E17 E70:E1048576 E19:E34 E48:E50 E52:E54 E36:E46 E64:E68 E56:E62</xm:sqref>
+          <xm:sqref>E1:E4 E6:E11 E13:E17 E72:E1048576 E19:E34 E48:E50 E52:E54 E36:E46 E66:E70 E56:E64</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>